<commit_message>
added note to BOM
</commit_message>
<xml_diff>
--- a/Hardware/tinyK22_Master/BOM TinyK22 Master.xlsx
+++ b/Hardware/tinyK22_Master/BOM TinyK22 Master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erich\Data\GitRepos\MetaClockClock\Hardware\tinyK22_Master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA22827C-9610-4487-8525-37288AA8823A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54158BB-D7DF-4FD4-9AFC-3850B25C1716}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25875" yWindow="-6270" windowWidth="25320" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25320" yWindow="-13290" windowWidth="18345" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>NOT the one on the board!</t>
-  </si>
-  <si>
     <t>Adafruit TSL2591</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>www.pcbway.com</t>
+  </si>
+  <si>
+    <t>NOT the one on the board! Check the BOM for PCBWay</t>
   </si>
 </sst>
 </file>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,8 @@
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
-    <col min="5" max="6" width="25" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -628,13 +629,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -652,13 +653,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -675,11 +676,11 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -697,11 +698,11 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -719,13 +720,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -738,16 +739,16 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -759,16 +760,16 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -778,7 +779,7 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
@@ -855,7 +856,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>15</v>
@@ -881,7 +882,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
@@ -935,7 +936,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -952,11 +953,11 @@
         <v>0.1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -974,11 +975,11 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -996,11 +997,11 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1018,14 +1019,14 @@
         <v>1.34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1042,11 +1043,11 @@
         <v>0.2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1064,11 +1065,11 @@
         <v>0.2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1086,14 +1087,14 @@
         <v>7.23</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>

</xml_diff>